<commit_message>
Continue implementing data entry to Excel
</commit_message>
<xml_diff>
--- a/app/routes/generate-reports/.server/workbooks/report.xlsx
+++ b/app/routes/generate-reports/.server/workbooks/report.xlsx
@@ -1594,25 +1594,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1622,6 +1610,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2010,8 +2010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI273"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A103" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="P253" sqref="P253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2039,43 +2039,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T1" s="41" t="s">
+      <c r="T1" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="41"/>
+      <c r="U1" s="47"/>
     </row>
     <row r="2" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
     </row>
     <row r="3" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
     </row>
     <row r="4" spans="1:22" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
-      <c r="U4" s="42"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
     </row>
     <row r="5" spans="1:22" ht="47.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:22" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2096,12 +2096,12 @@
       <c r="G6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="44" t="s">
+      <c r="H6" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
       <c r="L6" s="43" t="s">
         <v>4</v>
       </c>
@@ -2110,7 +2110,7 @@
       <c r="O6" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="48" t="s">
+      <c r="P6" s="44" t="s">
         <v>21</v>
       </c>
       <c r="Q6" s="43" t="s">
@@ -2130,7 +2130,7 @@
       <c r="D7" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="43" t="s">
@@ -2159,7 +2159,7 @@
         <v>30</v>
       </c>
       <c r="O7" s="43"/>
-      <c r="P7" s="49"/>
+      <c r="P7" s="45"/>
       <c r="Q7" s="43" t="s">
         <v>31</v>
       </c>
@@ -2186,7 +2186,7 @@
       <c r="M8" s="43"/>
       <c r="N8" s="43"/>
       <c r="O8" s="43"/>
-      <c r="P8" s="50"/>
+      <c r="P8" s="46"/>
       <c r="Q8" s="5" t="s">
         <v>33</v>
       </c>
@@ -11952,7 +11952,7 @@
       <c r="K202" s="5"/>
       <c r="L202" s="3"/>
       <c r="M202" s="3">
-        <f t="shared" ref="M202:M252" si="13">L202</f>
+        <f t="shared" ref="M202:M253" si="13">L202</f>
         <v>0</v>
       </c>
       <c r="N202" s="3" t="s">
@@ -14505,7 +14505,10 @@
       <c r="J253" s="5"/>
       <c r="K253" s="5"/>
       <c r="L253" s="3"/>
-      <c r="M253" s="3"/>
+      <c r="M253" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
       <c r="N253" s="3" t="s">
         <v>60</v>
       </c>
@@ -15117,19 +15120,19 @@
       <c r="U265" s="14"/>
     </row>
     <row r="266" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A266" s="46" t="s">
+      <c r="A266" s="41" t="s">
         <v>378</v>
       </c>
-      <c r="B266" s="46"/>
-      <c r="C266" s="46"/>
-      <c r="D266" s="46"/>
-      <c r="E266" s="46"/>
-      <c r="F266" s="46"/>
-      <c r="G266" s="46"/>
-      <c r="H266" s="46"/>
-      <c r="I266" s="46"/>
-      <c r="J266" s="46"/>
-      <c r="K266" s="46"/>
+      <c r="B266" s="41"/>
+      <c r="C266" s="41"/>
+      <c r="D266" s="41"/>
+      <c r="E266" s="41"/>
+      <c r="F266" s="41"/>
+      <c r="G266" s="41"/>
+      <c r="H266" s="41"/>
+      <c r="I266" s="41"/>
+      <c r="J266" s="41"/>
+      <c r="K266" s="41"/>
       <c r="L266" s="3"/>
       <c r="M266" s="3">
         <f t="shared" si="17"/>
@@ -15245,19 +15248,19 @@
       <c r="E271" s="36"/>
       <c r="F271" s="36"/>
       <c r="G271" s="36"/>
-      <c r="H271" s="47" t="s">
+      <c r="H271" s="42" t="s">
         <v>381</v>
       </c>
-      <c r="I271" s="47"/>
-      <c r="J271" s="47"/>
-      <c r="K271" s="47"/>
-      <c r="L271" s="47"/>
-      <c r="M271" s="47"/>
-      <c r="N271" s="47"/>
-      <c r="O271" s="47"/>
-      <c r="P271" s="47"/>
-      <c r="Q271" s="47"/>
-      <c r="R271" s="47"/>
+      <c r="I271" s="42"/>
+      <c r="J271" s="42"/>
+      <c r="K271" s="42"/>
+      <c r="L271" s="42"/>
+      <c r="M271" s="42"/>
+      <c r="N271" s="42"/>
+      <c r="O271" s="42"/>
+      <c r="P271" s="42"/>
+      <c r="Q271" s="42"/>
+      <c r="R271" s="42"/>
       <c r="S271" s="36"/>
       <c r="T271" s="36"/>
       <c r="U271" s="36"/>
@@ -15324,18 +15327,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A266:K266"/>
-    <mergeCell ref="H271:R271"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="P6:P8"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
     <mergeCell ref="T1:U3"/>
     <mergeCell ref="A4:U4"/>
     <mergeCell ref="A6:A8"/>
@@ -15351,6 +15342,18 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="A266:K266"/>
+    <mergeCell ref="H271:R271"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="P6:P8"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:B141 B145:B262 B265">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>

</xml_diff>